<commit_message>
update std confidence interval
</commit_message>
<xml_diff>
--- a/RTSNet_ICASSP.xlsx
+++ b/RTSNet_ICASSP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xiaoy\Documents\学习\ETH硕士\科研\wireless_comm_AI\loeliger\paper\ICASSP\simulations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xiaoy\Documents\RTSNet_Journal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{762E5053-9748-480C-B20E-AAC9A48A2173}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46FF49CD-E765-4AFA-AF36-C6158474E26F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Linear" sheetId="2" r:id="rId1"/>
@@ -842,7 +842,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1126,9 +1126,9 @@
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="37.08984375" customWidth="1"/>
+    <col min="1" max="1" width="37.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1634,14 +1634,14 @@
       <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="45.08984375" customWidth="1"/>
-    <col min="2" max="2" width="20.81640625" customWidth="1"/>
-    <col min="3" max="3" width="11.26953125" customWidth="1"/>
-    <col min="4" max="4" width="29.26953125" customWidth="1"/>
-    <col min="5" max="5" width="11.26953125" customWidth="1"/>
-    <col min="6" max="6" width="12.36328125" customWidth="1"/>
+    <col min="1" max="1" width="45.109375" customWidth="1"/>
+    <col min="2" max="2" width="20.77734375" customWidth="1"/>
+    <col min="3" max="3" width="11.21875" customWidth="1"/>
+    <col min="4" max="4" width="29.21875" customWidth="1"/>
+    <col min="5" max="5" width="11.21875" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -2185,10 +2185,10 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="30.6328125" customWidth="1"/>
-    <col min="2" max="2" width="12.81640625" customWidth="1"/>
+    <col min="1" max="1" width="30.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:9">

</xml_diff>